<commit_message>
Fixing bug with agency
</commit_message>
<xml_diff>
--- a/out/output.xlsx
+++ b/out/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,6 +593,870 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Haneen Bilal</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>METROPOLITAN CAPITAL REAL ESTATE - SOLE PROPRIETORSHIP L.L.C.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Jordan</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>English, Arabic</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971522222147</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>tel:+971565097986</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ayman Gumaa</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Realty Real Estate</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Sudan</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>English, Arabic</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971507568744</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>tel:+971565118215</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Daniela Giannone</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Probima Centre FZ LLC- RAK</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Italy</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>English, French, Italian</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971569374836</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>tel:+971569374836</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Besmir Selmani</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Henry Wiltshire International</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Albania</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971521905505</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>tel:+971565157405</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Paula Svensson</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Probima Centre FZ LLC- RAK</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Sweden</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>English, French, German, Swedish, Norwegian</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971566918386</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>tel:+971566918386</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Niel Els</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Paragon Properties</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> South Africa</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>English, Afrikaans</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971566677440</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>tel:+971565151679</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Gwen De Vos</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>McCone Properties</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Belgium</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>English, French, German, Dutch</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971506047936</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>tel:+971506047936</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Igor Dordevic</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Rosenheim Luxury Properties</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Serbia</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>English, Russian, Serbian</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971585527673</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>tel:+971565080442</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Iurii Loenko</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>fam Properties - Branch 3</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Russia</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>English, Russian</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971569551551</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>tel:+97145420820</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Majeed Ibrahiim</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>AGCO PROPERTIES</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Syria</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>English, Arabic, German</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971556261089</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>tel:+971565057663</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Lewis Chambers</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Arabian Estates</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> United Kingdom</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971508326839</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>tel:+971565224201</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Sergey Golubev</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Rosenheim Luxury Properties</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Russia</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Russian</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971585527673</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>tel:+971565115897</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Muhammad Mansoor</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ANW Real Estate</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Pakistan</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>English, Hindi, Urdu</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971548886019</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>tel:+971548886019</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Daniel Walker</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>White &amp; Co Real Estate</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> United Kingdom</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971561421175</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>tel:+971565067839</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Ahmed Sheikh</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>McCone Properties</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Pakistan</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>English, Arabic, Urdu</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971505726539</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>tel:+971505726539</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Ahmed Magdi</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>McCone Properties</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Egypt</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>English, Arabic</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971523992781</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>tel:+971523992781</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Harry Warren</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Arabian Estates</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> United Kingdom</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971582836910</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>tel:+971565093010</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Pawan Nagpal</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>INSIGHT PROPERTIES L.L.C</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> India</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>English, Hindi, Urdu, Punjabi, Sindhi</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971506954512</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>tel:+971506954512</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Hassan Raza</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>HIGHLINE REAL ESTATE</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Pakistan</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>English, Hindi, Urdu</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971544323800</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>tel:+971565224163</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Samy Aichouche</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>P M P Real Estate L.L.C</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> France</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>English, Arabic, French, Spanish</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971509735188</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>tel:+971509735188</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Daniel Manzetti</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>White &amp; Co Real Estate</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Norway</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>English, Swedish, Norwegian</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971561421175</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>tel:+971565097647</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Sagal Mahamed Ahmed</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>fam Properties - Branch 2</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> United Kingdom</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>English, Somali</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971569551551</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>tel:+97142483632</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Ruben Swanepoel</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Paragon Properties</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> South Africa</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>English, Afrikaans</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971586055662</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>tel:+971543078359</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Gayrat Pereligin</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>luxe homes Real Estate</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Uzbekistan</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>English, Russian, Uzbek</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971585989717</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>tel:+971565070759</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Behnia Tavassoli</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Veer &amp; Sant Real Estate L.L.C.</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Iran</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>English, Persian/Farsi</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971502971523</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>tel:+971502971523</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Lorenz De Blok</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>McCone Properties</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Belgium</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971523992781</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>tel:+971523992781</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Liewe Rutten</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>McCone Properties</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Belgium</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>https://wa.me/+971523992781</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>tel:+971523992781</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>